<commit_message>
Expand on SD results for Tony w/ F-tests
</commit_message>
<xml_diff>
--- a/draft-02/manuscript_ver3-4/sd-of-residuals-w-and-wo-outliers.xlsx
+++ b/draft-02/manuscript_ver3-4/sd-of-residuals-w-and-wo-outliers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1229B1AD-6389-5B4D-9185-FF806669578D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AABB9-7479-F040-997B-7A3C046858CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16540"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sd-of-residuals-w-and-wo-outlie" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>DS</t>
   </si>
@@ -75,11 +75,77 @@
   <si>
     <t>MV</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.466</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.337</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All other GCFR-SWAFR comparisons: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.01</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -206,7 +272,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +450,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -576,12 +648,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -595,6 +664,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -949,11 +1030,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -967,201 +1048,212 @@
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="1.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="11" max="11" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:11">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>965.28729503194904</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>638.37698587611305</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
+      <c r="F5" s="3"/>
+      <c r="G5" s="8">
         <v>665.01669227496905</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4">
+      <c r="H5" s="3"/>
+      <c r="I5" s="8">
         <v>383.79310102008498</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>558.40948500263096</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>353.93076929915799</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4">
+      <c r="F6" s="3"/>
+      <c r="G6" s="8">
         <v>554.67920763353004</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4">
+      <c r="H6" s="3"/>
+      <c r="I6" s="8">
         <v>336.42885340761302</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+    <row r="7" spans="1:11">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>607.10177186706801</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <v>540.16949843310999</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>467.825802826244</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
         <v>437.30975150846899</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>387.00494175833501</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
         <v>337.31179360655801</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
         <v>343.84351462341402</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
         <v>299.518852067323</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+    <row r="10" spans="1:11">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>335.17229652894201</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <v>315.519035929479</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
         <v>233.44825894088399</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
         <v>222.597231636732</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>247.394864914263</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
         <v>230.05084730116499</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
         <v>198.35573980529</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
         <v>174.12887031053799</v>
       </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="I14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>